<commit_message>
Tidied up code, Excel template
</commit_message>
<xml_diff>
--- a/storage/app/templates/kinerja_template.xlsx
+++ b/storage/app/templates/kinerja_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pmo-project\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C31451-5950-4DF4-ACDE-FF539D548868}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D1889A-5871-4CFA-9D97-CD48F8EB3EE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated template data types
</commit_message>
<xml_diff>
--- a/storage/app/templates/kinerja_template.xlsx
+++ b/storage/app/templates/kinerja_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\pmo-project\storage\app\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D1889A-5871-4CFA-9D97-CD48F8EB3EE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,27 +157,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +208,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{772ED741-8BC8-4D31-8B5E-BAF02F1F66F1}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -515,7 +510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -528,27 +523,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="100.7109375" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>